<commit_message>
Fit writing ats frame times
</commit_message>
<xml_diff>
--- a/ir_tools/data_formats/meta_data_record/Record_of_IRCAM_Velox_81kL_0102A_Operating_Settings.xlsx
+++ b/ir_tools/data_formats/meta_data_record/Record_of_IRCAM_Velox_81kL_0102A_Operating_Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\repos\ir_tools\ir_tools\data_formats\meta_data_record\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63419F3F-A140-4B7A-BD3A-4AACB067C912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAF3ABF-EB4E-42AE-B974-6A2ABF3BDC9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IRCAM Velox_81kL_0102A18CH_FAST" sheetId="1" r:id="rId1"/>
@@ -593,10 +593,10 @@
   <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="I48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="M66" sqref="M66:N66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>